<commit_message>
changed implementation for memory calculation
</commit_message>
<xml_diff>
--- a/src/main/resources/data_output/ParallelExecutionTimes.xlsx
+++ b/src/main/resources/data_output/ParallelExecutionTimes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anul1 IS1.1 Semestrul2\MEvPerf\SearchAlgorithms\src\main\resources\data_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F56159F-5D94-4A87-B539-21AB3835EBFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA16ADD0-99B3-4EF8-8CF6-031EDDA29682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,8 +62,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -91,8 +99,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,9 +416,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -427,53 +438,108 @@
     <col min="12" max="12" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2.5024199E-2</v>
+      </c>
+      <c r="B2">
+        <v>0.22209229999999999</v>
+      </c>
       <c r="C2">
         <v>4.3602000000000002E-2</v>
       </c>
       <c r="D2">
         <v>6.6455100000000003E-2</v>
+      </c>
+      <c r="E2">
+        <v>5.34846E-2</v>
+      </c>
+      <c r="F2">
+        <v>5.9721400000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2.6847900000000001E-2</v>
+      </c>
+      <c r="B3">
+        <v>1.3003199999999999E-2</v>
+      </c>
+      <c r="C3">
+        <v>5.5263999999999999E-3</v>
+      </c>
+      <c r="D3">
+        <v>7.3711999999999996E-3</v>
+      </c>
+      <c r="E3">
+        <v>5.2746000000000001E-2</v>
+      </c>
+      <c r="F3">
+        <v>5.6979200000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>7.9994000000000003E-3</v>
+      </c>
+      <c r="B4">
+        <v>2.2897500000000001E-2</v>
+      </c>
+      <c r="C4">
+        <v>2.6107999999999999E-3</v>
+      </c>
+      <c r="D4">
+        <v>2.5787000000000002E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>3.7161999999999998E-3</v>
+      </c>
+      <c r="D5">
+        <v>2.7705999999999998E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
display sequential data for graph and tree
</commit_message>
<xml_diff>
--- a/src/main/resources/data_output/ParallelExecutionTimes.xlsx
+++ b/src/main/resources/data_output/ParallelExecutionTimes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anul1 IS1.1 Semestrul2\MEvPerf\SearchAlgorithms\src\main\resources\data_output\"/>
     </mc:Choice>
@@ -62,6 +62,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
@@ -424,18 +425,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
-    <col min="7" max="7" width="17.21875" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.6640625"/>
+    <col min="2" max="2" customWidth="true" width="18.5546875"/>
+    <col min="3" max="3" customWidth="true" width="17.5546875"/>
+    <col min="4" max="4" customWidth="true" width="16.5546875"/>
+    <col min="5" max="5" customWidth="true" width="17.5546875"/>
+    <col min="6" max="6" customWidth="true" width="17.88671875"/>
+    <col min="7" max="7" customWidth="true" width="17.21875"/>
+    <col min="8" max="8" customWidth="true" width="18.21875"/>
+    <col min="9" max="9" customWidth="true" width="15.0"/>
+    <col min="10" max="10" customWidth="true" width="15.6640625"/>
+    <col min="11" max="11" customWidth="true" width="16.33203125"/>
+    <col min="12" max="12" customWidth="true" width="16.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -536,6 +537,14 @@
       </c>
       <c r="D5">
         <v>2.7705999999999998E-3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="n">
+        <v>0.0013182</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0014017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
display parallel data for tree
</commit_message>
<xml_diff>
--- a/src/main/resources/data_output/ParallelExecutionTimes.xlsx
+++ b/src/main/resources/data_output/ParallelExecutionTimes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anul1 IS1.1 Semestrul2\MEvPerf\SearchAlgorithms\src\main\resources\data_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA16ADD0-99B3-4EF8-8CF6-031EDDA29682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84995C13-B09F-49BE-A453-8211FB3D5DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Execution Times" sheetId="1" r:id="rId1"/>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,74 +477,46 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2.5024199E-2</v>
-      </c>
-      <c r="B2">
-        <v>0.22209229999999999</v>
-      </c>
-      <c r="C2">
-        <v>4.3602000000000002E-2</v>
-      </c>
-      <c r="D2">
-        <v>6.6455100000000003E-2</v>
-      </c>
-      <c r="E2">
-        <v>5.34846E-2</v>
-      </c>
-      <c r="F2">
-        <v>5.9721400000000001E-2</v>
+    <row r="2">
+      <c r="C2" t="n">
+        <v>0.0207863</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0256373</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1.315E-4</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3.602E-4</v>
+      </c>
+      <c r="I2" t="n">
+        <v>4.385E-4</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1.274E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2.6847900000000001E-2</v>
-      </c>
-      <c r="B3">
-        <v>1.3003199999999999E-2</v>
-      </c>
-      <c r="C3">
-        <v>5.5263999999999999E-3</v>
-      </c>
-      <c r="D3">
-        <v>7.3711999999999996E-3</v>
-      </c>
-      <c r="E3">
-        <v>5.2746000000000001E-2</v>
-      </c>
-      <c r="F3">
-        <v>5.6979200000000001E-2</v>
+    <row r="3">
+      <c r="G3" t="n">
+        <v>8.679E-4</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.0010293</v>
+      </c>
+      <c r="I3" t="n">
+        <v>3.156E-4</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2.806E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>7.9994000000000003E-3</v>
-      </c>
-      <c r="B4">
-        <v>2.2897500000000001E-2</v>
-      </c>
-      <c r="C4">
-        <v>2.6107999999999999E-3</v>
-      </c>
-      <c r="D4">
-        <v>2.5787000000000002E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C5">
-        <v>3.7161999999999998E-3</v>
-      </c>
-      <c r="D5">
-        <v>2.7705999999999998E-3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="C6" t="n">
-        <v>0.0013182</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.0014017</v>
+    <row r="4">
+      <c r="I4" t="n">
+        <v>3.374E-4</v>
+      </c>
+      <c r="J4" t="n">
+        <v>5.466E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed output for parallel tree execution
</commit_message>
<xml_diff>
--- a/src/main/resources/data_output/ParallelExecutionTimes.xlsx
+++ b/src/main/resources/data_output/ParallelExecutionTimes.xlsx
@@ -516,6 +516,12 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="n">
+        <v>0.0090386</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.0193585</v>
+      </c>
       <c r="C3" t="n">
         <v>0.0047659</v>
       </c>

</xml_diff>

<commit_message>
final output data and upgraded diagrams
</commit_message>
<xml_diff>
--- a/src/main/resources/data_output/ParallelExecutionTimes.xlsx
+++ b/src/main/resources/data_output/ParallelExecutionTimes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anul1 IS1.1 Semestrul2\MEvPerf\SearchAlgorithms\src\main\resources\data_output\"/>
     </mc:Choice>
@@ -62,6 +62,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6628,7 +6629,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="M28" sqref="M28"/>
@@ -6636,18 +6637,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
-    <col min="7" max="7" width="17.21875" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.6640625"/>
+    <col min="2" max="2" customWidth="true" width="18.5546875"/>
+    <col min="3" max="3" customWidth="true" width="17.5546875"/>
+    <col min="4" max="4" customWidth="true" width="16.5546875"/>
+    <col min="5" max="5" customWidth="true" width="17.5546875"/>
+    <col min="6" max="6" customWidth="true" width="17.88671875"/>
+    <col min="7" max="7" customWidth="true" width="17.21875"/>
+    <col min="8" max="8" customWidth="true" width="18.21875"/>
+    <col min="9" max="9" customWidth="true" width="15.0"/>
+    <col min="10" max="10" customWidth="true" width="15.6640625"/>
+    <col min="11" max="11" customWidth="true" width="16.33203125"/>
+    <col min="12" max="12" customWidth="true" width="16.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -7066,6 +7067,28 @@
       </c>
       <c r="L11" s="2">
         <v>3.191E-4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" t="n">
+        <v>0.006205</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0010974</v>
+      </c>
+      <c r="K12" t="n">
+        <v>2.724E-4</v>
+      </c>
+      <c r="L12" t="n">
+        <v>4.16E-4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" t="n">
+        <v>0.0022576</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.005929</v>
       </c>
     </row>
   </sheetData>

</xml_diff>